<commit_message>
better-organize xlsx Scenario data CAVESIM cases and presentation 20191106
</commit_message>
<xml_diff>
--- a/Data/Misc_Data_For_CAVESimV10_cases_and_report20191106.xlsx
+++ b/Data/Misc_Data_For_CAVESimV10_cases_and_report20191106.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pzl/Documents/Papers/2013AutomatedVehicles/2016CAVEnergyModel/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{62A75AA1-D131-5347-A0BA-D4CDE7A57537}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{49C4AD94-1731-4A48-9D34-3312AE5316D8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="960" windowWidth="27020" windowHeight="16540" activeTab="1" xr2:uid="{7415CC4D-CF24-9249-8F76-7F24CBAB6216}"/>
+    <workbookView xWindow="8820" yWindow="900" windowWidth="27020" windowHeight="16540" xr2:uid="{7415CC4D-CF24-9249-8F76-7F24CBAB6216}"/>
   </bookViews>
   <sheets>
     <sheet name="DemandParams" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="57">
   <si>
     <t>Underserved travelers</t>
   </si>
@@ -198,6 +198,12 @@
   </si>
   <si>
     <t>='[SMART_FY19_Scenario_Common_Assumptions_ 190821_v4_Basic_Reformatted.xlsx]SMART_FY19_Scenario_Common_Assu'!O6</t>
+  </si>
+  <si>
+    <t>----------</t>
+  </si>
+  <si>
+    <t>Rough estmations of power requirement vs speed, based only on assumed constant energy use per mile</t>
   </si>
 </sst>
 </file>
@@ -607,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D8FFA0B-B673-F643-9342-21DFCEBE403C}">
-  <dimension ref="A2:M27"/>
+  <dimension ref="A2:M29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -693,44 +699,44 @@
       </c>
     </row>
     <row r="8" spans="1:13">
-      <c r="A8" t="s">
-        <v>20</v>
+      <c r="A8" s="7" t="s">
+        <v>55</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="C8">
-        <v>2035</v>
+      <c r="C8" s="7" t="s">
+        <v>55</v>
       </c>
       <c r="D8" t="s">
         <v>23</v>
       </c>
-      <c r="E8" t="s">
-        <v>0</v>
+      <c r="E8" s="7" t="s">
+        <v>55</v>
       </c>
       <c r="F8" t="s">
         <v>23</v>
       </c>
-      <c r="G8">
-        <v>0</v>
+      <c r="G8" s="7" t="s">
+        <v>55</v>
       </c>
       <c r="H8" t="s">
         <v>23</v>
       </c>
-      <c r="I8">
-        <v>6</v>
+      <c r="I8" s="7" t="s">
+        <v>55</v>
       </c>
       <c r="J8" t="s">
         <v>23</v>
       </c>
-      <c r="K8">
-        <v>10</v>
+      <c r="K8" s="7" t="s">
+        <v>55</v>
       </c>
       <c r="L8" t="s">
         <v>23</v>
       </c>
-      <c r="M8">
-        <v>0</v>
+      <c r="M8" s="7" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:13">
@@ -747,25 +753,25 @@
         <v>23</v>
       </c>
       <c r="E9" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F9" t="s">
         <v>23</v>
       </c>
       <c r="G9">
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="H9" t="s">
         <v>23</v>
       </c>
       <c r="I9">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="J9" t="s">
         <v>23</v>
       </c>
       <c r="K9">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="L9" t="s">
         <v>23</v>
@@ -788,25 +794,25 @@
         <v>23</v>
       </c>
       <c r="E10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="F10" t="s">
         <v>23</v>
       </c>
       <c r="G10">
-        <v>15</v>
+        <v>-20</v>
       </c>
       <c r="H10" t="s">
         <v>23</v>
       </c>
       <c r="I10">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="J10" t="s">
         <v>23</v>
       </c>
       <c r="K10">
-        <v>67</v>
+        <v>50</v>
       </c>
       <c r="L10" t="s">
         <v>23</v>
@@ -823,31 +829,31 @@
         <v>23</v>
       </c>
       <c r="C11">
-        <v>2050</v>
+        <v>2035</v>
       </c>
       <c r="D11" t="s">
         <v>23</v>
       </c>
       <c r="E11" t="s">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="F11" t="s">
         <v>23</v>
       </c>
       <c r="G11">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="H11" t="s">
         <v>23</v>
       </c>
       <c r="I11">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="J11" t="s">
         <v>23</v>
       </c>
       <c r="K11">
-        <v>10</v>
+        <v>67</v>
       </c>
       <c r="L11" t="s">
         <v>23</v>
@@ -870,25 +876,25 @@
         <v>23</v>
       </c>
       <c r="E12" t="s">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="F12" t="s">
         <v>23</v>
       </c>
       <c r="G12">
-        <v>-20</v>
+        <v>0</v>
       </c>
       <c r="H12" t="s">
         <v>23</v>
       </c>
       <c r="I12">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="J12" t="s">
         <v>23</v>
       </c>
       <c r="K12">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="L12" t="s">
         <v>23</v>
@@ -911,188 +917,369 @@
         <v>23</v>
       </c>
       <c r="E13" t="s">
+        <v>16</v>
+      </c>
+      <c r="F13" t="s">
+        <v>23</v>
+      </c>
+      <c r="G13">
+        <v>-20</v>
+      </c>
+      <c r="H13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I13">
+        <v>30</v>
+      </c>
+      <c r="J13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13">
+        <v>50</v>
+      </c>
+      <c r="L13" t="s">
+        <v>23</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14">
+        <v>2050</v>
+      </c>
+      <c r="D14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E14" t="s">
         <v>15</v>
       </c>
-      <c r="F13" t="s">
-        <v>23</v>
-      </c>
-      <c r="G13">
+      <c r="F14" t="s">
+        <v>23</v>
+      </c>
+      <c r="G14">
         <v>15</v>
       </c>
-      <c r="H13" t="s">
-        <v>23</v>
-      </c>
-      <c r="I13">
+      <c r="H14" t="s">
+        <v>23</v>
+      </c>
+      <c r="I14">
         <v>25</v>
       </c>
-      <c r="J13" t="s">
-        <v>23</v>
-      </c>
-      <c r="K13">
+      <c r="J14" t="s">
+        <v>23</v>
+      </c>
+      <c r="K14">
         <v>67</v>
       </c>
-      <c r="L13" t="s">
-        <v>23</v>
-      </c>
-      <c r="M13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" s="1" customFormat="1">
-      <c r="A15" s="1" t="s">
-        <v>32</v>
+      <c r="L14" t="s">
+        <v>23</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:13" s="1" customFormat="1">
       <c r="A16" s="1" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="1" customFormat="1">
       <c r="A17" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="I17" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>1</v>
+        <v>12</v>
       </c>
     </row>
     <row r="18" spans="1:11" s="1" customFormat="1">
       <c r="A18" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F18" t="s">
+        <v>23</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H18" t="s">
+        <v>23</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J18" t="s">
+        <v>23</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="1" customFormat="1">
+      <c r="A19" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" t="s">
+        <v>23</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="D19" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" t="s">
+        <v>23</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="H19" t="s">
+        <v>23</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="J19" t="s">
+        <v>23</v>
+      </c>
+      <c r="K19" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="1" customFormat="1">
+      <c r="A20" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="1" t="s">
+      <c r="B20" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="E18" s="1">
-        <v>0</v>
-      </c>
-      <c r="G18" s="1">
+      <c r="D20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="1">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" s="1">
         <v>-0.2</v>
       </c>
-      <c r="I18" s="1">
+      <c r="H20" t="s">
+        <v>23</v>
+      </c>
+      <c r="I20" s="1">
         <v>0.3</v>
       </c>
-      <c r="K18" s="1">
+      <c r="J20" t="s">
+        <v>23</v>
+      </c>
+      <c r="K20" s="1">
         <v>0.3</v>
       </c>
     </row>
-    <row r="19" spans="1:11" s="1" customFormat="1">
-      <c r="A19" s="1" t="s">
+    <row r="21" spans="1:11" s="1" customFormat="1">
+      <c r="A21" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="B21" t="s">
+        <v>23</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E19" s="1">
-        <v>0</v>
-      </c>
-      <c r="G19" s="1">
+      <c r="D21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" s="1">
+        <v>0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>23</v>
+      </c>
+      <c r="G21" s="1">
         <v>-0.2</v>
       </c>
-      <c r="I19" s="1">
+      <c r="H21" t="s">
+        <v>23</v>
+      </c>
+      <c r="I21" s="1">
         <v>0.3</v>
       </c>
-      <c r="K19" s="1">
+      <c r="J21" t="s">
+        <v>23</v>
+      </c>
+      <c r="K21" s="1">
         <v>0.3</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11">
-      <c r="A20" t="s">
-        <v>7</v>
-      </c>
-      <c r="C20" t="s">
-        <v>10</v>
-      </c>
-      <c r="E20">
-        <v>0</v>
-      </c>
-      <c r="G20">
-        <v>-0.2</v>
-      </c>
-      <c r="I20">
-        <v>0.3</v>
-      </c>
-      <c r="K20">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11">
-      <c r="A21" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" t="s">
-        <v>8</v>
-      </c>
-      <c r="E21">
-        <v>0</v>
-      </c>
-      <c r="G21">
-        <v>0</v>
-      </c>
-      <c r="I21">
-        <v>0</v>
-      </c>
-      <c r="K21">
-        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:11">
       <c r="A22" t="s">
-        <v>11</v>
+        <v>7</v>
+      </c>
+      <c r="B22" t="s">
+        <v>23</v>
       </c>
       <c r="C22" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="D22" t="s">
+        <v>23</v>
       </c>
       <c r="E22">
         <v>0</v>
       </c>
+      <c r="F22" t="s">
+        <v>23</v>
+      </c>
       <c r="G22">
-        <v>0</v>
+        <v>-0.2</v>
+      </c>
+      <c r="H22" t="s">
+        <v>23</v>
       </c>
       <c r="I22">
-        <v>0</v>
+        <v>0.3</v>
+      </c>
+      <c r="J22" t="s">
+        <v>23</v>
       </c>
       <c r="K22">
-        <v>0</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="23" spans="1:11">
       <c r="A23" t="s">
         <v>11</v>
       </c>
+      <c r="B23" t="s">
+        <v>23</v>
+      </c>
       <c r="C23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" t="s">
+        <v>23</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23" t="s">
+        <v>23</v>
+      </c>
+      <c r="G23">
+        <v>0</v>
+      </c>
+      <c r="H23" t="s">
+        <v>23</v>
+      </c>
+      <c r="I23">
+        <v>0</v>
+      </c>
+      <c r="J23" t="s">
+        <v>23</v>
+      </c>
+      <c r="K23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11">
+      <c r="A24" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" t="s">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" t="s">
+        <v>23</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>23</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24" t="s">
+        <v>23</v>
+      </c>
+      <c r="I24">
+        <v>0</v>
+      </c>
+      <c r="J24" t="s">
+        <v>23</v>
+      </c>
+      <c r="K24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11">
+      <c r="A25" t="s">
+        <v>11</v>
+      </c>
+      <c r="B25" t="s">
+        <v>23</v>
+      </c>
+      <c r="C25" t="s">
         <v>10</v>
       </c>
-      <c r="E23">
-        <v>0</v>
-      </c>
-      <c r="G23">
-        <v>0</v>
-      </c>
-      <c r="I23">
+      <c r="D25" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>23</v>
+      </c>
+      <c r="G25">
+        <v>0</v>
+      </c>
+      <c r="H25" t="s">
+        <v>23</v>
+      </c>
+      <c r="I25">
         <v>0.3</v>
       </c>
-      <c r="K23">
+      <c r="J25" t="s">
+        <v>23</v>
+      </c>
+      <c r="K25">
         <v>0.6</v>
       </c>
     </row>
-    <row r="27" spans="1:11">
-      <c r="A27" t="s">
+    <row r="29" spans="1:11">
+      <c r="A29" t="s">
         <v>14</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C29" t="s">
         <v>13</v>
       </c>
     </row>
@@ -1105,8 +1292,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49BE9BFC-DF11-D443-BCAE-6F5931495360}">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2:G2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1321,14 +1508,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D3C4125-D7C5-E84C-A6D8-7C206FC3081E}">
-  <dimension ref="A3:B11"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>56</v>
+      </c>
+    </row>
     <row r="3" spans="1:2">
       <c r="A3" t="s">
         <v>26</v>

</xml_diff>